<commit_message>
Actualizar archivos de output con correcciones y agregar .gitignore
- Agregado .gitignore para archivos Python (__pycache__, *.pyc, etc)
- Actualizado dashboard_2025_11.html con alertas dinámicas
- Actualizado reporte_ejecutivo_2025_11.xlsx con hoja "Top Egresos"

Los archivos de output fueron regenerados con las correcciones implementadas.
</commit_message>
<xml_diff>
--- a/output/reporte_ejecutivo_2025_11.xlsx
+++ b/output/reporte_ejecutivo_2025_11.xlsx
@@ -10,8 +10,9 @@
     <sheet name="Resumen" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Ingresos" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Egresos" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Prestadores" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sin Clasificar" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Top Egresos" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Prestadores" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sin Clasificar" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -678,100 +679,76 @@
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Pacientes Transferencia</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>$0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25"/>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>DESGLOSE EGRESOS</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Monto</t>
+        </is>
+      </c>
+    </row>
     <row r="26">
-      <c r="A26" s="5" t="inlineStr">
-        <is>
-          <t>DESGLOSE EGRESOS</t>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Comisiones Bancarias</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Monto</t>
+          <t>$330,101.89</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Comisiones Bancarias</t>
+          <t>Gastos Operativos</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>$330,101.89</t>
+          <t>$1,581,480.67</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gastos Operativos</t>
+          <t>Impuestos</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>$1,581,480.67</t>
+          <t>$500,006.05</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Impuestos</t>
+          <t>Prestadores</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$500,006.05</t>
+          <t>$6,356,029.00</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Prestadores</t>
+          <t>Servicios</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>$6,356,029.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Servicios</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
           <t>$492,236.40</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Sueldos</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -12596,6 +12573,381 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Ranking</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Concepto</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Detalle</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Monto</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Subcategoría</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Banco</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>45945.77690972222</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>45939.78494212963</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>862300</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>45954.57414351852</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>600000</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>45954.57196759259</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>600000</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>45954.57053240741</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>600000</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>45950.68238425926</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>375000</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>45939.82627314814</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>350000</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>45950.68052083333</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>304500</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>45938.59410879629</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Compra Visa Débito</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>COMERCIO: PAGOS360*EPEC OPERACION: 139928</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>239243.1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Servicios</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>45938.48383101852</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>CONCEPTO: Transferencia enviada TERMINAL: TESP0000...</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>204254</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Prestadores</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Supervielle</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12761,7 +13113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>